<commit_message>
Add May Session Analysis
</commit_message>
<xml_diff>
--- a/df_head.xlsx
+++ b/df_head.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Mombo ShotID</t>
+          <t>Mombo_ShotID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -466,137 +466,137 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Ball (mph)</t>
+          <t>Ball_mph</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Club (mph)</t>
+          <t>Club_mph</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Smash Factor</t>
+          <t>Smash_Factor</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Carry (yds)</t>
+          <t>Carry_yds</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Total (yds)</t>
+          <t>Total_yds</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Roll (yds)</t>
+          <t>Roll_yds</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Swing H (°)*</t>
+          <t>Swing_H</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Spin (rpm)</t>
+          <t>Spin_rpm</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Height (ft)</t>
+          <t>Height_ft</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Time (s)</t>
+          <t>Time_s</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>AOA (°)*</t>
+          <t>AOA</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Spin Loft (°)</t>
+          <t>Spin_Loft</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Swing V (°)*</t>
+          <t>Swing_V</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Spin Axis (°)</t>
+          <t>Spin_Axis</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Lateral (yds)</t>
+          <t>Lateral_yds</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Shot Type</t>
+          <t>Shot_Type</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>FTP (°)</t>
+          <t>FTP</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>FTT (°)</t>
+          <t>FTT</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Dynamic Loft (°)</t>
+          <t>Dynamic_Loft</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Club Path (°)</t>
+          <t>Club_Path</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Launch H (°)</t>
+          <t>Launch_H</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Launch V (°)</t>
+          <t>Launch_V</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>Low Point (ftin)</t>
+          <t>Low_Point_ftin</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>DescentV (°)</t>
+          <t>DescentV</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>Curve Dist (yds)</t>
+          <t>Curve_Dist_yds</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>Lateral Impact (in)</t>
+          <t>Lateral_Impact_in</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>Vertical Impact (in)</t>
+          <t>Vertical_Impact_in</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
@@ -611,32 +611,32 @@
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 35</t>
+          <t>Unnamed_35</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 36</t>
+          <t>Unnamed_36</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 37</t>
+          <t>Unnamed_37</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 38</t>
+          <t>Unnamed_38</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 39</t>
+          <t>Unnamed_39</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 40</t>
+          <t>Unnamed_40</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
@@ -724,8 +724,10 @@
       <c r="S2" t="n">
         <v>67</v>
       </c>
-      <c r="T2" t="n">
-        <v>13.8</v>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>13.8 L</t>
+        </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
@@ -755,16 +757,16 @@
           <t>1.3 R</t>
         </is>
       </c>
-      <c r="AA2" t="n">
-        <v>4.9</v>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>4.9 L</t>
+        </is>
       </c>
       <c r="AB2" t="n">
         <v>18.9</v>
       </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>4.6″</t>
-        </is>
+      <c r="AC2" t="n">
+        <v>4.6</v>
       </c>
       <c r="AD2" t="n">
         <v>40.3</v>
@@ -857,8 +859,10 @@
       <c r="S3" t="n">
         <v>66.09999999999999</v>
       </c>
-      <c r="T3" t="n">
-        <v>9.5</v>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>9.5 L</t>
+        </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
@@ -888,16 +892,16 @@
           <t>0.2 R</t>
         </is>
       </c>
-      <c r="AA3" t="n">
-        <v>4.2</v>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>4.2 L</t>
+        </is>
       </c>
       <c r="AB3" t="n">
         <v>18.6</v>
       </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>5.9″</t>
-        </is>
+      <c r="AC3" t="n">
+        <v>5.9</v>
       </c>
       <c r="AD3" t="n">
         <v>32.2</v>
@@ -990,8 +994,10 @@
       <c r="S4" t="n">
         <v>63.4</v>
       </c>
-      <c r="T4" t="n">
-        <v>7.3</v>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>7.3 L</t>
+        </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
@@ -1021,16 +1027,16 @@
           <t>1.6 L</t>
         </is>
       </c>
-      <c r="AA4" t="n">
-        <v>4.8</v>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>4.8 L</t>
+        </is>
       </c>
       <c r="AB4" t="n">
         <v>19.1</v>
       </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>5.3″</t>
-        </is>
+      <c r="AC4" t="n">
+        <v>5.3</v>
       </c>
       <c r="AD4" t="n">
         <v>34.7</v>
@@ -1123,8 +1129,10 @@
       <c r="S5" t="n">
         <v>63.8</v>
       </c>
-      <c r="T5" t="n">
-        <v>12.2</v>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>12.2 L</t>
+        </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
@@ -1154,16 +1162,16 @@
           <t>1.3 L</t>
         </is>
       </c>
-      <c r="AA5" t="n">
-        <v>6.6</v>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>6.6 L</t>
+        </is>
       </c>
       <c r="AB5" t="n">
         <v>17.7</v>
       </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>4.6″</t>
-        </is>
+      <c r="AC5" t="n">
+        <v>4.6</v>
       </c>
       <c r="AD5" t="n">
         <v>29.9</v>
@@ -1256,8 +1264,10 @@
       <c r="S6" t="n">
         <v>67.09999999999999</v>
       </c>
-      <c r="T6" t="n">
-        <v>3.3</v>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>3.3 L</t>
+        </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
@@ -1287,16 +1297,16 @@
           <t>3.3 L</t>
         </is>
       </c>
-      <c r="AA6" t="n">
-        <v>4.9</v>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>4.9 L</t>
+        </is>
       </c>
       <c r="AB6" t="n">
         <v>20.2</v>
       </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>5.2″</t>
-        </is>
+      <c r="AC6" t="n">
+        <v>5.2</v>
       </c>
       <c r="AD6" t="n">
         <v>34</v>

</xml_diff>